<commit_message>
updated data dictionary to include Answer column
</commit_message>
<xml_diff>
--- a/references/sample-data-dictionary.xlsx
+++ b/references/sample-data-dictionary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Data Element</t>
   </si>
@@ -169,13 +169,22 @@
   </si>
   <si>
     <t>Ordinal</t>
+  </si>
+  <si>
+    <t>Answers</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Follow up email with request for rating</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +218,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -251,7 +266,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -291,6 +306,7 @@
     <xf numFmtId="15" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -607,13 +623,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,15 +641,15 @@
     <col min="7" max="7" width="9.6640625" style="8" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" style="9" customWidth="1"/>
     <col min="9" max="9" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="34.21875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="34.33203125" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="2"/>
+    <col min="10" max="12" width="34.21875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="34.33203125" style="5" customWidth="1"/>
+    <col min="20" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -664,28 +680,31 @@
       <c r="J1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q1"/>
       <c r="R1"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>28</v>
       </c>
@@ -711,21 +730,22 @@
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
-      <c r="L2" s="10">
+      <c r="L2" s="10"/>
+      <c r="M2" s="10">
         <v>1000080</v>
       </c>
-      <c r="M2" s="10">
+      <c r="N2" s="10">
         <v>1000081</v>
       </c>
-      <c r="N2" s="10">
+      <c r="O2" s="10">
         <v>1000082</v>
       </c>
-      <c r="O2" s="10"/>
       <c r="P2" s="10"/>
-      <c r="Q2"/>
+      <c r="Q2" s="10"/>
       <c r="R2"/>
-    </row>
-    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S2"/>
+    </row>
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>31</v>
       </c>
@@ -752,24 +772,25 @@
         <v>34</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="10"/>
+      <c r="L3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="10">
+      <c r="M3" s="10">
         <v>402</v>
       </c>
-      <c r="M3" s="10">
+      <c r="N3" s="10">
         <v>300</v>
       </c>
-      <c r="N3" s="10">
+      <c r="O3" s="10">
         <v>690</v>
       </c>
-      <c r="O3" s="10"/>
       <c r="P3" s="10"/>
-      <c r="Q3"/>
+      <c r="Q3" s="10"/>
       <c r="R3"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>35</v>
       </c>
@@ -796,22 +817,25 @@
       <c r="J4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="15">
+      <c r="K4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="15">
         <v>113.05</v>
       </c>
-      <c r="M4" s="16">
+      <c r="N4" s="16">
         <v>160.55000000000001</v>
       </c>
-      <c r="N4" s="16">
+      <c r="O4" s="16">
         <v>200.69</v>
       </c>
-      <c r="O4" s="10"/>
       <c r="P4" s="10"/>
-      <c r="Q4"/>
+      <c r="Q4" s="10"/>
       <c r="R4"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>38</v>
       </c>
@@ -839,21 +863,22 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="10"/>
+      <c r="M5" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="N5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="O5" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O5" s="10"/>
       <c r="P5" s="10"/>
-      <c r="Q5"/>
+      <c r="Q5" s="10"/>
       <c r="R5"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S5"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>40</v>
       </c>
@@ -884,22 +909,25 @@
       <c r="J6" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10">
+      <c r="K6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10">
         <v>4</v>
       </c>
-      <c r="M6" s="10">
+      <c r="N6" s="10">
         <v>9</v>
       </c>
-      <c r="N6" s="10">
+      <c r="O6" s="10">
         <v>5</v>
       </c>
-      <c r="O6" s="10"/>
       <c r="P6" s="10"/>
-      <c r="Q6"/>
+      <c r="Q6" s="10"/>
       <c r="R6"/>
-    </row>
-    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S6"/>
+    </row>
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
@@ -911,15 +939,16 @@
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="14"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="17"/>
       <c r="N7" s="14"/>
-      <c r="O7" s="10"/>
+      <c r="O7" s="14"/>
       <c r="P7" s="10"/>
-      <c r="Q7"/>
+      <c r="Q7" s="10"/>
       <c r="R7"/>
-    </row>
-    <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S7"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -931,15 +960,16 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="17"/>
       <c r="P8" s="10"/>
-      <c r="Q8"/>
+      <c r="Q8" s="10"/>
       <c r="R8"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S8"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
@@ -951,15 +981,16 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="15"/>
+      <c r="L9" s="10"/>
       <c r="M9" s="15"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="10"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="16"/>
       <c r="P9" s="10"/>
-      <c r="Q9"/>
+      <c r="Q9" s="10"/>
       <c r="R9"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S9"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
@@ -971,13 +1002,14 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="15"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
-      <c r="O10" s="10"/>
+      <c r="O10" s="15"/>
       <c r="P10" s="10"/>
-      <c r="Q10"/>
+      <c r="Q10" s="10"/>
       <c r="R10"/>
+      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>